<commit_message>
detecting R peaks from NST database
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/AHA.xlsx
+++ b/R peak detection/beatdetection/AHA.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="sheet1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>1627</v>
+        <v>1650</v>
       </c>
       <c r="C1" t="n">
         <v>1622</v>
@@ -456,7 +456,7 @@
         <v>1621</v>
       </c>
       <c r="E1" t="n">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="F1" t="n">
         <v>0</v>
@@ -465,13 +465,13 @@
         <v>100</v>
       </c>
       <c r="H1" t="n">
-        <v>99.69249692496925</v>
+        <v>98.30200121285628</v>
       </c>
       <c r="I1" t="n">
-        <v>0.003082614056720099</v>
+        <v>0.01726263871763255</v>
       </c>
       <c r="J1" t="n">
-        <v>64.36959052085876</v>
+        <v>139.6599147319794</v>
       </c>
     </row>
     <row r="2">
@@ -505,7 +505,7 @@
         <v>0.0003853564547206166</v>
       </c>
       <c r="J2" t="n">
-        <v>65.98829102516174</v>
+        <v>120.9806885719299</v>
       </c>
     </row>
     <row r="3">
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2182</v>
+        <v>2184</v>
       </c>
       <c r="C3" t="n">
         <v>2181</v>
@@ -524,7 +524,7 @@
         <v>2180</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -533,13 +533,13 @@
         <v>100</v>
       </c>
       <c r="H3" t="n">
-        <v>99.95414947271894</v>
+        <v>99.86257443884563</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0004585052728106373</v>
+        <v>0.001375515818431912</v>
       </c>
       <c r="J3" t="n">
-        <v>64.40073037147522</v>
+        <v>169.744309425354</v>
       </c>
     </row>
     <row r="4">
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2947</v>
+        <v>2948</v>
       </c>
       <c r="C4" t="n">
         <v>2974</v>
@@ -558,7 +558,7 @@
         <v>2943</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
         <v>30</v>
@@ -567,13 +567,13 @@
         <v>98.99091826437942</v>
       </c>
       <c r="H4" t="n">
-        <v>99.89816700610999</v>
+        <v>99.86426874787919</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01109616677874916</v>
+        <v>0.01143241425689307</v>
       </c>
       <c r="J4" t="n">
-        <v>67.18800663948059</v>
+        <v>102.4175889492035</v>
       </c>
     </row>
     <row r="5">
@@ -607,7 +607,7 @@
         <v>0.0003915426781519186</v>
       </c>
       <c r="J5" t="n">
-        <v>63.75170564651489</v>
+        <v>153.27952003479</v>
       </c>
     </row>
     <row r="6">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2123</v>
+        <v>2124</v>
       </c>
       <c r="C6" t="n">
         <v>2122</v>
@@ -626,7 +626,7 @@
         <v>2121</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -635,13 +635,13 @@
         <v>100</v>
       </c>
       <c r="H6" t="n">
-        <v>99.95287464655985</v>
+        <v>99.90579368817711</v>
       </c>
       <c r="I6" t="n">
-        <v>0.000471253534401508</v>
+        <v>0.000942507068803016</v>
       </c>
       <c r="J6" t="n">
-        <v>64.5881290435791</v>
+        <v>173.5799686908722</v>
       </c>
     </row>
     <row r="7">
@@ -675,7 +675,7 @@
         <v>0.0006510416666666666</v>
       </c>
       <c r="J7" t="n">
-        <v>63.11406755447388</v>
+        <v>171.8458025455475</v>
       </c>
     </row>
     <row r="8">
@@ -709,7 +709,7 @@
         <v>0.0004084967320261438</v>
       </c>
       <c r="J8" t="n">
-        <v>65.33007192611694</v>
+        <v>181.4454717636108</v>
       </c>
     </row>
     <row r="9">
@@ -743,7 +743,7 @@
         <v>0.0002791736460078169</v>
       </c>
       <c r="J9" t="n">
-        <v>66.52996706962585</v>
+        <v>87.44014072418213</v>
       </c>
     </row>
     <row r="10">
@@ -753,31 +753,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2015</v>
+        <v>2198</v>
       </c>
       <c r="C10" t="n">
         <v>1997</v>
       </c>
       <c r="D10" t="n">
-        <v>1985</v>
+        <v>1992</v>
       </c>
       <c r="E10" t="n">
-        <v>29</v>
+        <v>205</v>
       </c>
       <c r="F10" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G10" t="n">
-        <v>99.44889779559118</v>
+        <v>99.79959919839679</v>
       </c>
       <c r="H10" t="n">
-        <v>98.56007944389275</v>
+        <v>90.66909421939008</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0200300450676014</v>
+        <v>0.1046569854782173</v>
       </c>
       <c r="J10" t="n">
-        <v>66.17162203788757</v>
+        <v>193.4952464103699</v>
       </c>
     </row>
     <row r="11">
@@ -811,7 +811,7 @@
         <v>0.0003478260869565218</v>
       </c>
       <c r="J11" t="n">
-        <v>65.60803484916687</v>
+        <v>85.12370324134827</v>
       </c>
     </row>
     <row r="12">
@@ -821,7 +821,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2415</v>
+        <v>2416</v>
       </c>
       <c r="C12" t="n">
         <v>2414</v>
@@ -830,7 +830,7 @@
         <v>2413</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -839,13 +839,13 @@
         <v>100</v>
       </c>
       <c r="H12" t="n">
-        <v>99.95857497928749</v>
+        <v>99.91718426501035</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0004142502071251035</v>
+        <v>0.0008285004142502071</v>
       </c>
       <c r="J12" t="n">
-        <v>64.68193769454956</v>
+        <v>184.5667395591736</v>
       </c>
     </row>
     <row r="13">
@@ -855,31 +855,31 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3389</v>
+        <v>3448</v>
       </c>
       <c r="C13" t="n">
         <v>3511</v>
       </c>
       <c r="D13" t="n">
-        <v>3380</v>
+        <v>3432</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F13" t="n">
-        <v>130</v>
+        <v>78</v>
       </c>
       <c r="G13" t="n">
-        <v>96.29629629629629</v>
+        <v>97.77777777777777</v>
       </c>
       <c r="H13" t="n">
-        <v>99.76387249114522</v>
+        <v>99.56483899042645</v>
       </c>
       <c r="I13" t="n">
-        <v>0.03930504129877527</v>
+        <v>0.02648818000569638</v>
       </c>
       <c r="J13" t="n">
-        <v>68.59865140914917</v>
+        <v>90.92623424530029</v>
       </c>
     </row>
     <row r="14">
@@ -889,31 +889,31 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1666</v>
+        <v>1678</v>
       </c>
       <c r="C14" t="n">
         <v>1628</v>
       </c>
       <c r="D14" t="n">
-        <v>1626</v>
+        <v>1627</v>
       </c>
       <c r="E14" t="n">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>99.93853718500307</v>
+        <v>100</v>
       </c>
       <c r="H14" t="n">
-        <v>97.65765765765765</v>
+        <v>97.01848539057842</v>
       </c>
       <c r="I14" t="n">
-        <v>0.02457002457002457</v>
+        <v>0.03071253071253071</v>
       </c>
       <c r="J14" t="n">
-        <v>64.50711512565613</v>
+        <v>200.5196526050568</v>
       </c>
     </row>
     <row r="15">
@@ -923,7 +923,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1620</v>
+        <v>1621</v>
       </c>
       <c r="C15" t="n">
         <v>1613</v>
@@ -932,7 +932,7 @@
         <v>1612</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -941,13 +941,13 @@
         <v>100</v>
       </c>
       <c r="H15" t="n">
-        <v>99.56763434218654</v>
+        <v>99.50617283950618</v>
       </c>
       <c r="I15" t="n">
-        <v>0.004339739615623063</v>
+        <v>0.004959702417854928</v>
       </c>
       <c r="J15" t="n">
-        <v>63.45167589187622</v>
+        <v>197.74587059021</v>
       </c>
     </row>
     <row r="16">
@@ -981,7 +981,7 @@
         <v>0.000608457560085184</v>
       </c>
       <c r="J16" t="n">
-        <v>66.44238710403442</v>
+        <v>82.84662389755249</v>
       </c>
     </row>
     <row r="17">
@@ -1015,7 +1015,7 @@
         <v>0.000350385423966363</v>
       </c>
       <c r="J17" t="n">
-        <v>67.70910906791687</v>
+        <v>97.6238694190979</v>
       </c>
     </row>
     <row r="18">
@@ -1049,7 +1049,7 @@
         <v>0.0004139072847682119</v>
       </c>
       <c r="J18" t="n">
-        <v>65.37798810005188</v>
+        <v>221.4122416973114</v>
       </c>
     </row>
     <row r="19">
@@ -1059,7 +1059,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2535</v>
+        <v>2536</v>
       </c>
       <c r="C19" t="n">
         <v>2537</v>
@@ -1068,7 +1068,7 @@
         <v>2533</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>3</v>
@@ -1077,13 +1077,13 @@
         <v>99.88170347003154</v>
       </c>
       <c r="H19" t="n">
-        <v>99.96053670086819</v>
+        <v>99.92110453648915</v>
       </c>
       <c r="I19" t="n">
-        <v>0.001576665352778873</v>
+        <v>0.001970831690973591</v>
       </c>
       <c r="J19" t="n">
-        <v>65.41233944892883</v>
+        <v>194.3023428916931</v>
       </c>
     </row>
     <row r="20">
@@ -1117,7 +1117,7 @@
         <v>0.003674781809830041</v>
       </c>
       <c r="J20" t="n">
-        <v>64.2497820854187</v>
+        <v>258.834000825882</v>
       </c>
     </row>
     <row r="21">
@@ -1127,31 +1127,31 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2942</v>
+        <v>2944</v>
       </c>
       <c r="C21" t="n">
         <v>2943</v>
       </c>
       <c r="D21" t="n">
-        <v>2940</v>
+        <v>2942</v>
       </c>
       <c r="E21" t="n">
         <v>1</v>
       </c>
       <c r="F21" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>99.93201903467029</v>
+        <v>100</v>
       </c>
       <c r="H21" t="n">
-        <v>99.9659979598776</v>
+        <v>99.9660210669385</v>
       </c>
       <c r="I21" t="n">
-        <v>0.001019367991845056</v>
+        <v>0.0003397893306150187</v>
       </c>
       <c r="J21" t="n">
-        <v>65.3978283405304</v>
+        <v>86.70143127441406</v>
       </c>
     </row>
     <row r="22">
@@ -1161,7 +1161,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1955</v>
+        <v>1958</v>
       </c>
       <c r="C22" t="n">
         <v>1950</v>
@@ -1170,7 +1170,7 @@
         <v>1949</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -1179,13 +1179,13 @@
         <v>100</v>
       </c>
       <c r="H22" t="n">
-        <v>99.74411463664278</v>
+        <v>99.59121103730199</v>
       </c>
       <c r="I22" t="n">
-        <v>0.002564102564102564</v>
+        <v>0.004102564102564103</v>
       </c>
       <c r="J22" t="n">
-        <v>63.55813264846802</v>
+        <v>263.9532952308655</v>
       </c>
     </row>
     <row r="23">
@@ -1219,7 +1219,7 @@
         <v>0.001064962726304579</v>
       </c>
       <c r="J23" t="n">
-        <v>66.81389021873474</v>
+        <v>261.3846805095673</v>
       </c>
     </row>
     <row r="24">
@@ -1229,7 +1229,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1785</v>
+        <v>1786</v>
       </c>
       <c r="C24" t="n">
         <v>1784</v>
@@ -1238,7 +1238,7 @@
         <v>1781</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>2</v>
@@ -1247,13 +1247,13 @@
         <v>99.88782950084128</v>
       </c>
       <c r="H24" t="n">
-        <v>99.83183856502242</v>
+        <v>99.77591036414566</v>
       </c>
       <c r="I24" t="n">
-        <v>0.002802690582959641</v>
+        <v>0.00336322869955157</v>
       </c>
       <c r="J24" t="n">
-        <v>65.41823148727417</v>
+        <v>272.2939174175262</v>
       </c>
     </row>
     <row r="25">
@@ -1287,7 +1287,7 @@
         <v>0.0006163328197226503</v>
       </c>
       <c r="J25" t="n">
-        <v>64.22615957260132</v>
+        <v>85.41774153709412</v>
       </c>
     </row>
     <row r="26">
@@ -1297,7 +1297,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2324</v>
+        <v>2326</v>
       </c>
       <c r="C26" t="n">
         <v>2324</v>
@@ -1306,7 +1306,7 @@
         <v>2322</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>1</v>
@@ -1315,13 +1315,13 @@
         <v>99.95695221696083</v>
       </c>
       <c r="H26" t="n">
-        <v>99.95695221696083</v>
+        <v>99.87096774193549</v>
       </c>
       <c r="I26" t="n">
-        <v>0.0008605851979345956</v>
+        <v>0.001721170395869191</v>
       </c>
       <c r="J26" t="n">
-        <v>66.66014742851257</v>
+        <v>299.3385264873505</v>
       </c>
     </row>
     <row r="27">
@@ -1331,7 +1331,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2425</v>
+        <v>2426</v>
       </c>
       <c r="C27" t="n">
         <v>2424</v>
@@ -1340,7 +1340,7 @@
         <v>2423</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -1349,13 +1349,13 @@
         <v>100</v>
       </c>
       <c r="H27" t="n">
-        <v>99.95874587458746</v>
+        <v>99.91752577319588</v>
       </c>
       <c r="I27" t="n">
-        <v>0.0004125412541254125</v>
+        <v>0.0008250825082508251</v>
       </c>
       <c r="J27" t="n">
-        <v>64.02292227745056</v>
+        <v>219.5192229747772</v>
       </c>
     </row>
     <row r="28">
@@ -1365,7 +1365,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2585</v>
+        <v>2588</v>
       </c>
       <c r="C28" t="n">
         <v>2584</v>
@@ -1374,7 +1374,7 @@
         <v>2583</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
@@ -1383,13 +1383,13 @@
         <v>100</v>
       </c>
       <c r="H28" t="n">
-        <v>99.96130030959752</v>
+        <v>99.84538074990336</v>
       </c>
       <c r="I28" t="n">
-        <v>0.0003869969040247678</v>
+        <v>0.001547987616099071</v>
       </c>
       <c r="J28" t="n">
-        <v>64.94367933273315</v>
+        <v>164.9190139770508</v>
       </c>
     </row>
     <row r="29">
@@ -1399,7 +1399,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>2445</v>
+        <v>2446</v>
       </c>
       <c r="C29" t="n">
         <v>2472</v>
@@ -1408,7 +1408,7 @@
         <v>2443</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>28</v>
@@ -1417,13 +1417,13 @@
         <v>98.86685552407933</v>
       </c>
       <c r="H29" t="n">
-        <v>99.95908346972176</v>
+        <v>99.91820040899796</v>
       </c>
       <c r="I29" t="n">
-        <v>0.01173139158576052</v>
+        <v>0.01213592233009709</v>
       </c>
       <c r="J29" t="n">
-        <v>65.62935328483582</v>
+        <v>271.4453647136688</v>
       </c>
     </row>
     <row r="30">
@@ -1457,7 +1457,7 @@
         <v>0.0005175983436853002</v>
       </c>
       <c r="J30" t="n">
-        <v>63.38640689849854</v>
+        <v>273.0712873935699</v>
       </c>
     </row>
     <row r="31">
@@ -1467,31 +1467,31 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2346</v>
+        <v>2351</v>
       </c>
       <c r="C31" t="n">
         <v>2376</v>
       </c>
       <c r="D31" t="n">
-        <v>2344</v>
+        <v>2345</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G31" t="n">
-        <v>98.69473684210526</v>
+        <v>98.73684210526316</v>
       </c>
       <c r="H31" t="n">
-        <v>99.95735607675905</v>
+        <v>99.78723404255319</v>
       </c>
       <c r="I31" t="n">
-        <v>0.01346801346801347</v>
+        <v>0.01473063973063973</v>
       </c>
       <c r="J31" t="n">
-        <v>64.46110963821411</v>
+        <v>295.9710457324982</v>
       </c>
     </row>
     <row r="32">
@@ -1525,7 +1525,7 @@
         <v>0.0003872966692486445</v>
       </c>
       <c r="J32" t="n">
-        <v>64.56665873527527</v>
+        <v>225.4252634048462</v>
       </c>
     </row>
     <row r="33">
@@ -1535,7 +1535,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>2259</v>
+        <v>2263</v>
       </c>
       <c r="C33" t="n">
         <v>2258</v>
@@ -1544,7 +1544,7 @@
         <v>2257</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
@@ -1553,13 +1553,13 @@
         <v>100</v>
       </c>
       <c r="H33" t="n">
-        <v>99.95571302037202</v>
+        <v>99.7789566755084</v>
       </c>
       <c r="I33" t="n">
-        <v>0.0004428697962798937</v>
+        <v>0.002214348981399469</v>
       </c>
       <c r="J33" t="n">
-        <v>64.44725584983826</v>
+        <v>349.5846335887909</v>
       </c>
     </row>
     <row r="34">
@@ -1569,7 +1569,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1448</v>
+        <v>1450</v>
       </c>
       <c r="C34" t="n">
         <v>1452</v>
@@ -1578,7 +1578,7 @@
         <v>1445</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>6</v>
@@ -1587,13 +1587,13 @@
         <v>99.58649207443143</v>
       </c>
       <c r="H34" t="n">
-        <v>99.86178299930891</v>
+        <v>99.72394755003451</v>
       </c>
       <c r="I34" t="n">
-        <v>0.005509641873278237</v>
+        <v>0.006887052341597796</v>
       </c>
       <c r="J34" t="n">
-        <v>63.11000061035156</v>
+        <v>281.9280273914337</v>
       </c>
     </row>
     <row r="35">
@@ -1603,7 +1603,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1829</v>
+        <v>1830</v>
       </c>
       <c r="C35" t="n">
         <v>1947</v>
@@ -1612,7 +1612,7 @@
         <v>1827</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>119</v>
@@ -1621,13 +1621,13 @@
         <v>93.88489208633094</v>
       </c>
       <c r="H35" t="n">
-        <v>99.945295404814</v>
+        <v>99.89065062875889</v>
       </c>
       <c r="I35" t="n">
-        <v>0.06163328197226502</v>
+        <v>0.06214689265536723</v>
       </c>
       <c r="J35" t="n">
-        <v>63.12672185897827</v>
+        <v>344.356076002121</v>
       </c>
     </row>
     <row r="36">
@@ -1637,31 +1637,31 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>3518</v>
+        <v>3525</v>
       </c>
       <c r="C36" t="n">
         <v>3520</v>
       </c>
       <c r="D36" t="n">
-        <v>3512</v>
+        <v>3516</v>
       </c>
       <c r="E36" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F36" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G36" t="n">
-        <v>99.80107985223074</v>
+        <v>99.9147485080989</v>
       </c>
       <c r="H36" t="n">
-        <v>99.85783338072221</v>
+        <v>99.77298524404087</v>
       </c>
       <c r="I36" t="n">
-        <v>0.003409090909090909</v>
+        <v>0.003125</v>
       </c>
       <c r="J36" t="n">
-        <v>68.24345970153809</v>
+        <v>102.2146134376526</v>
       </c>
     </row>
     <row r="37">
@@ -1671,7 +1671,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1882</v>
+        <v>1889</v>
       </c>
       <c r="C37" t="n">
         <v>1878</v>
@@ -1680,7 +1680,7 @@
         <v>1877</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F37" t="n">
         <v>0</v>
@@ -1689,13 +1689,13 @@
         <v>100</v>
       </c>
       <c r="H37" t="n">
-        <v>99.7873471557682</v>
+        <v>99.41737288135593</v>
       </c>
       <c r="I37" t="n">
-        <v>0.002129925452609159</v>
+        <v>0.005857294994675187</v>
       </c>
       <c r="J37" t="n">
-        <v>64.70016312599182</v>
+        <v>357.3414137363434</v>
       </c>
     </row>
     <row r="38">
@@ -1729,7 +1729,7 @@
         <v>0.002952340784479123</v>
       </c>
       <c r="J38" t="n">
-        <v>64.81442403793335</v>
+        <v>303.3961703777313</v>
       </c>
     </row>
     <row r="39">
@@ -1739,31 +1739,31 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2874</v>
+        <v>2875</v>
       </c>
       <c r="C39" t="n">
         <v>2907</v>
       </c>
       <c r="D39" t="n">
-        <v>2872</v>
+        <v>2873</v>
       </c>
       <c r="E39" t="n">
         <v>1</v>
       </c>
       <c r="F39" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G39" t="n">
-        <v>98.83000688231246</v>
+        <v>98.86441844459739</v>
       </c>
       <c r="H39" t="n">
-        <v>99.96519317786286</v>
+        <v>99.9652052887961</v>
       </c>
       <c r="I39" t="n">
-        <v>0.01203990368077055</v>
+        <v>0.01169590643274854</v>
       </c>
       <c r="J39" t="n">
-        <v>64.5556333065033</v>
+        <v>157.624972820282</v>
       </c>
     </row>
     <row r="40">
@@ -1773,31 +1773,31 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>2025</v>
+        <v>2033</v>
       </c>
       <c r="C40" t="n">
         <v>2257</v>
       </c>
       <c r="D40" t="n">
-        <v>2021</v>
+        <v>2028</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="G40" t="n">
-        <v>89.58333333333333</v>
+        <v>89.8936170212766</v>
       </c>
       <c r="H40" t="n">
-        <v>99.85177865612648</v>
+        <v>99.80314960629921</v>
       </c>
       <c r="I40" t="n">
-        <v>0.1054497120070891</v>
+        <v>0.10279131590607</v>
       </c>
       <c r="J40" t="n">
-        <v>64.08829689025879</v>
+        <v>398.2216620445251</v>
       </c>
     </row>
     <row r="41">
@@ -1807,31 +1807,31 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2345</v>
+        <v>2352</v>
       </c>
       <c r="C41" t="n">
         <v>2351</v>
       </c>
       <c r="D41" t="n">
-        <v>2341</v>
+        <v>2348</v>
       </c>
       <c r="E41" t="n">
         <v>3</v>
       </c>
       <c r="F41" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G41" t="n">
-        <v>99.61702127659575</v>
+        <v>99.91489361702128</v>
       </c>
       <c r="H41" t="n">
-        <v>99.87201365187714</v>
+        <v>99.87239472564866</v>
       </c>
       <c r="I41" t="n">
-        <v>0.005104210974053594</v>
+        <v>0.002126754572522331</v>
       </c>
       <c r="J41" t="n">
-        <v>64.3602340221405</v>
+        <v>400.3833718299866</v>
       </c>
     </row>
     <row r="42">
@@ -1841,7 +1841,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>2374</v>
+        <v>2408</v>
       </c>
       <c r="C42" t="n">
         <v>2374</v>
@@ -1850,7 +1850,7 @@
         <v>2372</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="F42" t="n">
         <v>1</v>
@@ -1859,13 +1859,13 @@
         <v>99.95785924989465</v>
       </c>
       <c r="H42" t="n">
-        <v>99.95785924989465</v>
+        <v>98.54590776900706</v>
       </c>
       <c r="I42" t="n">
-        <v>0.0008424599831508003</v>
+        <v>0.01516427969671441</v>
       </c>
       <c r="J42" t="n">
-        <v>65.374844789505</v>
+        <v>518.8608622550964</v>
       </c>
     </row>
     <row r="43">
@@ -1875,7 +1875,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>2288</v>
+        <v>2289</v>
       </c>
       <c r="C43" t="n">
         <v>2287</v>
@@ -1884,7 +1884,7 @@
         <v>2286</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
@@ -1893,13 +1893,13 @@
         <v>100</v>
       </c>
       <c r="H43" t="n">
-        <v>99.95627459554001</v>
+        <v>99.91258741258741</v>
       </c>
       <c r="I43" t="n">
-        <v>0.0004372540445999126</v>
+        <v>0.0008745080891998251</v>
       </c>
       <c r="J43" t="n">
-        <v>63.84267830848694</v>
+        <v>463.520263671875</v>
       </c>
     </row>
     <row r="44">
@@ -1933,7 +1933,7 @@
         <v>0.0005537098560354374</v>
       </c>
       <c r="J44" t="n">
-        <v>63.1483416557312</v>
+        <v>420.813549041748</v>
       </c>
     </row>
     <row r="45">
@@ -1943,7 +1943,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>2070</v>
+        <v>2089</v>
       </c>
       <c r="C45" t="n">
         <v>2068</v>
@@ -1952,7 +1952,7 @@
         <v>2066</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="F45" t="n">
         <v>1</v>
@@ -1961,13 +1961,13 @@
         <v>99.95162070633769</v>
       </c>
       <c r="H45" t="n">
-        <v>99.85500241662639</v>
+        <v>98.94636015325671</v>
       </c>
       <c r="I45" t="n">
-        <v>0.001934235976789168</v>
+        <v>0.01112185686653772</v>
       </c>
       <c r="J45" t="n">
-        <v>65.18136143684387</v>
+        <v>444.3889617919922</v>
       </c>
     </row>
     <row r="46">
@@ -2001,7 +2001,7 @@
         <v>0.0006842285323297981</v>
       </c>
       <c r="J46" t="n">
-        <v>66.06016397476196</v>
+        <v>209.5371160507202</v>
       </c>
     </row>
     <row r="47">
@@ -2011,7 +2011,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>1846</v>
+        <v>1874</v>
       </c>
       <c r="C47" t="n">
         <v>1845</v>
@@ -2020,7 +2020,7 @@
         <v>1844</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F47" t="n">
         <v>0</v>
@@ -2029,13 +2029,13 @@
         <v>100</v>
       </c>
       <c r="H47" t="n">
-        <v>99.94579945799458</v>
+        <v>98.45168179391351</v>
       </c>
       <c r="I47" t="n">
-        <v>0.0005420054200542005</v>
+        <v>0.01571815718157182</v>
       </c>
       <c r="J47" t="n">
-        <v>64.60397243499756</v>
+        <v>393.7255070209503</v>
       </c>
     </row>
     <row r="48">
@@ -2045,31 +2045,31 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2158</v>
+        <v>2167</v>
       </c>
       <c r="C48" t="n">
         <v>2164</v>
       </c>
       <c r="D48" t="n">
-        <v>2156</v>
+        <v>2163</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>99.67637540453075</v>
+        <v>100</v>
       </c>
       <c r="H48" t="n">
-        <v>99.95363931386184</v>
+        <v>99.86149584487535</v>
       </c>
       <c r="I48" t="n">
-        <v>0.003696857670979667</v>
+        <v>0.001386321626617375</v>
       </c>
       <c r="J48" t="n">
-        <v>63.50957202911377</v>
+        <v>448.1733231544495</v>
       </c>
     </row>
     <row r="49">
@@ -2079,7 +2079,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>2019</v>
+        <v>2051</v>
       </c>
       <c r="C49" t="n">
         <v>2017</v>
@@ -2088,7 +2088,7 @@
         <v>2016</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="F49" t="n">
         <v>0</v>
@@ -2097,13 +2097,13 @@
         <v>100</v>
       </c>
       <c r="H49" t="n">
-        <v>99.90089197224975</v>
+        <v>98.34146341463415</v>
       </c>
       <c r="I49" t="n">
-        <v>0.0009915716410510659</v>
+        <v>0.01685671789786812</v>
       </c>
       <c r="J49" t="n">
-        <v>70.10827589035034</v>
+        <v>427.775475025177</v>
       </c>
     </row>
     <row r="50">
@@ -2113,31 +2113,31 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>2497</v>
+        <v>2502</v>
       </c>
       <c r="C50" t="n">
         <v>2501</v>
       </c>
       <c r="D50" t="n">
-        <v>2495</v>
+        <v>2500</v>
       </c>
       <c r="E50" t="n">
         <v>1</v>
       </c>
       <c r="F50" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>99.8</v>
+        <v>100</v>
       </c>
       <c r="H50" t="n">
-        <v>99.9599358974359</v>
+        <v>99.96001599360255</v>
       </c>
       <c r="I50" t="n">
-        <v>0.002399040383846461</v>
+        <v>0.0003998400639744102</v>
       </c>
       <c r="J50" t="n">
-        <v>69.20495676994324</v>
+        <v>478.1130404472351</v>
       </c>
     </row>
     <row r="51">
@@ -2171,7 +2171,7 @@
         <v>0.001024065540194572</v>
       </c>
       <c r="J51" t="n">
-        <v>64.8571310043335</v>
+        <v>429.7898063659668</v>
       </c>
     </row>
     <row r="52">
@@ -2181,31 +2181,31 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>2697</v>
+        <v>2698</v>
       </c>
       <c r="C52" t="n">
         <v>2698</v>
       </c>
       <c r="D52" t="n">
-        <v>2695</v>
+        <v>2696</v>
       </c>
       <c r="E52" t="n">
         <v>1</v>
       </c>
       <c r="F52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G52" t="n">
-        <v>99.92584352984798</v>
+        <v>99.96292176492399</v>
       </c>
       <c r="H52" t="n">
-        <v>99.96290801186943</v>
+        <v>99.96292176492399</v>
       </c>
       <c r="I52" t="n">
-        <v>0.001111934766493699</v>
+        <v>0.0007412898443291327</v>
       </c>
       <c r="J52" t="n">
-        <v>63.85849475860596</v>
+        <v>175.7156212329865</v>
       </c>
     </row>
     <row r="53">
@@ -2215,31 +2215,31 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>2246</v>
+        <v>2252</v>
       </c>
       <c r="C53" t="n">
         <v>2251</v>
       </c>
       <c r="D53" t="n">
-        <v>2244</v>
+        <v>2250</v>
       </c>
       <c r="E53" t="n">
         <v>1</v>
       </c>
       <c r="F53" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>99.73333333333333</v>
+        <v>100</v>
       </c>
       <c r="H53" t="n">
-        <v>99.9554565701559</v>
+        <v>99.95557529986672</v>
       </c>
       <c r="I53" t="n">
-        <v>0.003109729009329187</v>
+        <v>0.000444247001332741</v>
       </c>
       <c r="J53" t="n">
-        <v>64.51595377922058</v>
+        <v>391.7056906223297</v>
       </c>
     </row>
     <row r="54">
@@ -2249,31 +2249,31 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>2295</v>
+        <v>2296</v>
       </c>
       <c r="C54" t="n">
         <v>2294</v>
       </c>
       <c r="D54" t="n">
-        <v>2292</v>
+        <v>2293</v>
       </c>
       <c r="E54" t="n">
         <v>2</v>
       </c>
       <c r="F54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54" t="n">
-        <v>99.95638901003053</v>
+        <v>100</v>
       </c>
       <c r="H54" t="n">
-        <v>99.9128160418483</v>
+        <v>99.91285403050109</v>
       </c>
       <c r="I54" t="n">
-        <v>0.001307759372275501</v>
+        <v>0.0008718395815170009</v>
       </c>
       <c r="J54" t="n">
-        <v>64.85180640220642</v>
+        <v>457.4525661468506</v>
       </c>
     </row>
     <row r="55">
@@ -2307,7 +2307,7 @@
         <v>0.003590664272890485</v>
       </c>
       <c r="J55" t="n">
-        <v>66.91018581390381</v>
+        <v>105.1737875938416</v>
       </c>
     </row>
     <row r="56">
@@ -2317,7 +2317,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="C56" t="n">
         <v>2044</v>
@@ -2326,7 +2326,7 @@
         <v>2043</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>0</v>
@@ -2335,13 +2335,13 @@
         <v>100</v>
       </c>
       <c r="H56" t="n">
-        <v>99.95107632093934</v>
+        <v>99.90220048899755</v>
       </c>
       <c r="I56" t="n">
-        <v>0.0004892367906066536</v>
+        <v>0.0009784735812133072</v>
       </c>
       <c r="J56" t="n">
-        <v>64.63725352287292</v>
+        <v>415.654666185379</v>
       </c>
     </row>
     <row r="57">
@@ -2351,7 +2351,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>2360</v>
+        <v>2393</v>
       </c>
       <c r="C57" t="n">
         <v>2359</v>
@@ -2360,7 +2360,7 @@
         <v>2358</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="F57" t="n">
         <v>0</v>
@@ -2369,13 +2369,13 @@
         <v>100</v>
       </c>
       <c r="H57" t="n">
-        <v>99.95760915642221</v>
+        <v>98.57859531772576</v>
       </c>
       <c r="I57" t="n">
-        <v>0.000423908435777872</v>
+        <v>0.01441288681644765</v>
       </c>
       <c r="J57" t="n">
-        <v>64.61130166053772</v>
+        <v>528.8224492073059</v>
       </c>
     </row>
     <row r="58">
@@ -2385,7 +2385,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>2503</v>
+        <v>2504</v>
       </c>
       <c r="C58" t="n">
         <v>2500</v>
@@ -2394,7 +2394,7 @@
         <v>2499</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>0</v>
@@ -2403,13 +2403,13 @@
         <v>100</v>
       </c>
       <c r="H58" t="n">
-        <v>99.88009592326139</v>
+        <v>99.84019176987614</v>
       </c>
       <c r="I58" t="n">
-        <v>0.0012</v>
+        <v>0.0016</v>
       </c>
       <c r="J58" t="n">
-        <v>64.07124018669128</v>
+        <v>407.8547523021698</v>
       </c>
     </row>
     <row r="59">
@@ -2419,31 +2419,31 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>3273</v>
+        <v>3288</v>
       </c>
       <c r="C59" t="n">
         <v>3289</v>
       </c>
       <c r="D59" t="n">
-        <v>3271</v>
+        <v>3286</v>
       </c>
       <c r="E59" t="n">
         <v>1</v>
       </c>
       <c r="F59" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="G59" t="n">
-        <v>99.48296836982968</v>
+        <v>99.93917274939173</v>
       </c>
       <c r="H59" t="n">
-        <v>99.96943765281173</v>
+        <v>99.96957712199574</v>
       </c>
       <c r="I59" t="n">
-        <v>0.005472788081483734</v>
+        <v>0.0009121313469139556</v>
       </c>
       <c r="J59" t="n">
-        <v>67.16881465911865</v>
+        <v>100.7897553443909</v>
       </c>
     </row>
     <row r="60">
@@ -2453,31 +2453,31 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>3155</v>
+        <v>3159</v>
       </c>
       <c r="C60" t="n">
         <v>3164</v>
       </c>
       <c r="D60" t="n">
-        <v>3153</v>
+        <v>3157</v>
       </c>
       <c r="E60" t="n">
         <v>1</v>
       </c>
       <c r="F60" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G60" t="n">
-        <v>99.68384445147012</v>
+        <v>99.81030667088207</v>
       </c>
       <c r="H60" t="n">
-        <v>99.96829422954978</v>
+        <v>99.96833438885371</v>
       </c>
       <c r="I60" t="n">
-        <v>0.00347661188369153</v>
+        <v>0.002212389380530973</v>
       </c>
       <c r="J60" t="n">
-        <v>64.91057801246643</v>
+        <v>103.9685049057007</v>
       </c>
     </row>
     <row r="61">
@@ -2487,31 +2487,31 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>2128</v>
+        <v>2129</v>
       </c>
       <c r="C61" t="n">
         <v>2128</v>
       </c>
       <c r="D61" t="n">
-        <v>2126</v>
+        <v>2127</v>
       </c>
       <c r="E61" t="n">
         <v>1</v>
       </c>
       <c r="F61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>99.9529854254819</v>
+        <v>100</v>
       </c>
       <c r="H61" t="n">
-        <v>99.9529854254819</v>
+        <v>99.95300751879699</v>
       </c>
       <c r="I61" t="n">
-        <v>0.0009398496240601503</v>
+        <v>0.0004699248120300752</v>
       </c>
       <c r="J61" t="n">
-        <v>64.02824735641479</v>
+        <v>502.6864905357361</v>
       </c>
     </row>
     <row r="62">
@@ -2521,7 +2521,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>2534</v>
+        <v>2538</v>
       </c>
       <c r="C62" t="n">
         <v>2533</v>
@@ -2530,7 +2530,7 @@
         <v>2532</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>0</v>
@@ -2539,13 +2539,13 @@
         <v>100</v>
       </c>
       <c r="H62" t="n">
-        <v>99.96052112120016</v>
+        <v>99.80291683090265</v>
       </c>
       <c r="I62" t="n">
-        <v>0.0003947887879984208</v>
+        <v>0.001973943939992104</v>
       </c>
       <c r="J62" t="n">
-        <v>65.15616583824158</v>
+        <v>452.5304152965546</v>
       </c>
     </row>
     <row r="63">
@@ -2555,31 +2555,31 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>1919</v>
+        <v>1927</v>
       </c>
       <c r="C63" t="n">
         <v>1927</v>
       </c>
       <c r="D63" t="n">
-        <v>1916</v>
+        <v>1924</v>
       </c>
       <c r="E63" t="n">
         <v>2</v>
       </c>
       <c r="F63" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G63" t="n">
-        <v>99.48078920041537</v>
+        <v>99.89615784008308</v>
       </c>
       <c r="H63" t="n">
-        <v>99.89572471324296</v>
+        <v>99.89615784008308</v>
       </c>
       <c r="I63" t="n">
-        <v>0.006227296315516347</v>
+        <v>0.002075765438505449</v>
       </c>
       <c r="J63" t="n">
-        <v>64.00376391410828</v>
+        <v>508.5395138263702</v>
       </c>
     </row>
     <row r="64">
@@ -2589,31 +2589,31 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>2332</v>
+        <v>2456</v>
       </c>
       <c r="C64" t="n">
         <v>2437</v>
       </c>
       <c r="D64" t="n">
-        <v>2315</v>
+        <v>2422</v>
       </c>
       <c r="E64" t="n">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="F64" t="n">
-        <v>121</v>
+        <v>14</v>
       </c>
       <c r="G64" t="n">
-        <v>95.03284072249589</v>
+        <v>99.42528735632185</v>
       </c>
       <c r="H64" t="n">
-        <v>99.31359931359931</v>
+        <v>98.65580448065172</v>
       </c>
       <c r="I64" t="n">
-        <v>0.05621665982765695</v>
+        <v>0.01928600738613049</v>
       </c>
       <c r="J64" t="n">
-        <v>65.46449518203735</v>
+        <v>564.7112579345703</v>
       </c>
     </row>
     <row r="65">
@@ -2623,31 +2623,31 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>2870</v>
+        <v>3090</v>
       </c>
       <c r="C65" t="n">
         <v>3109</v>
       </c>
       <c r="D65" t="n">
-        <v>2868</v>
+        <v>3088</v>
       </c>
       <c r="E65" t="n">
         <v>1</v>
       </c>
       <c r="F65" t="n">
-        <v>240</v>
+        <v>20</v>
       </c>
       <c r="G65" t="n">
-        <v>92.27799227799228</v>
+        <v>99.35649935649936</v>
       </c>
       <c r="H65" t="n">
-        <v>99.96514464970373</v>
+        <v>99.96762706377469</v>
       </c>
       <c r="I65" t="n">
-        <v>0.07751688645866839</v>
+        <v>0.006754583467352846</v>
       </c>
       <c r="J65" t="n">
-        <v>65.79371118545532</v>
+        <v>325.2862832546234</v>
       </c>
     </row>
     <row r="66">
@@ -2657,31 +2657,31 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>2336</v>
+        <v>2351</v>
       </c>
       <c r="C66" t="n">
         <v>2340</v>
       </c>
       <c r="D66" t="n">
-        <v>2332</v>
+        <v>2336</v>
       </c>
       <c r="E66" t="n">
+        <v>14</v>
+      </c>
+      <c r="F66" t="n">
         <v>3</v>
       </c>
-      <c r="F66" t="n">
-        <v>7</v>
-      </c>
       <c r="G66" t="n">
-        <v>99.70072680632749</v>
+        <v>99.87174005985464</v>
       </c>
       <c r="H66" t="n">
-        <v>99.87152034261241</v>
+        <v>99.40425531914893</v>
       </c>
       <c r="I66" t="n">
-        <v>0.004273504273504274</v>
+        <v>0.007264957264957265</v>
       </c>
       <c r="J66" t="n">
-        <v>64.49150729179382</v>
+        <v>553.6992700099945</v>
       </c>
     </row>
     <row r="67">
@@ -2715,7 +2715,7 @@
         <v>0.0006389776357827476</v>
       </c>
       <c r="J67" t="n">
-        <v>62.76056814193726</v>
+        <v>459.8499341011047</v>
       </c>
     </row>
     <row r="68">
@@ -2725,31 +2725,31 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>2800</v>
+        <v>2899</v>
       </c>
       <c r="C68" t="n">
         <v>2897</v>
       </c>
       <c r="D68" t="n">
-        <v>2780</v>
+        <v>2876</v>
       </c>
       <c r="E68" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F68" t="n">
-        <v>116</v>
+        <v>20</v>
       </c>
       <c r="G68" t="n">
-        <v>95.99447513812154</v>
+        <v>99.30939226519337</v>
       </c>
       <c r="H68" t="n">
-        <v>99.32118613790639</v>
+        <v>99.24085576259489</v>
       </c>
       <c r="I68" t="n">
-        <v>0.04659993096306524</v>
+        <v>0.0144977562996203</v>
       </c>
       <c r="J68" t="n">
-        <v>65.78163361549377</v>
+        <v>340.652770280838</v>
       </c>
     </row>
     <row r="69">
@@ -2759,31 +2759,31 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>1787</v>
+        <v>1788</v>
       </c>
       <c r="C69" t="n">
         <v>1753</v>
       </c>
       <c r="D69" t="n">
-        <v>1751</v>
+        <v>1752</v>
       </c>
       <c r="E69" t="n">
         <v>35</v>
       </c>
       <c r="F69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>99.94292237442923</v>
+        <v>100</v>
       </c>
       <c r="H69" t="n">
-        <v>98.04031354983202</v>
+        <v>98.04141018466704</v>
       </c>
       <c r="I69" t="n">
-        <v>0.02053622361665716</v>
+        <v>0.0199657729606389</v>
       </c>
       <c r="J69" t="n">
-        <v>63.81159591674805</v>
+        <v>516.2697296142578</v>
       </c>
     </row>
     <row r="70">
@@ -2793,7 +2793,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>1850</v>
+        <v>1940</v>
       </c>
       <c r="C70" t="n">
         <v>1459</v>
@@ -2802,7 +2802,7 @@
         <v>1453</v>
       </c>
       <c r="E70" t="n">
-        <v>396</v>
+        <v>486</v>
       </c>
       <c r="F70" t="n">
         <v>5</v>
@@ -2811,13 +2811,13 @@
         <v>99.65706447187928</v>
       </c>
       <c r="H70" t="n">
-        <v>78.58301784748512</v>
+        <v>74.93553378029912</v>
       </c>
       <c r="I70" t="n">
-        <v>0.2748457847840987</v>
+        <v>0.3365318711446196</v>
       </c>
       <c r="J70" t="n">
-        <v>64.58599019050598</v>
+        <v>495.1612267494202</v>
       </c>
     </row>
     <row r="71">
@@ -2827,31 +2827,31 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>1865</v>
+        <v>1910</v>
       </c>
       <c r="C71" t="n">
         <v>1787</v>
       </c>
       <c r="D71" t="n">
-        <v>1737</v>
+        <v>1761</v>
       </c>
       <c r="E71" t="n">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="F71" t="n">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="G71" t="n">
-        <v>97.25643896976484</v>
+        <v>98.60022396416574</v>
       </c>
       <c r="H71" t="n">
-        <v>93.18669527896996</v>
+        <v>92.24724986904138</v>
       </c>
       <c r="I71" t="n">
-        <v>0.09848908785674315</v>
+        <v>0.09681029658645775</v>
       </c>
       <c r="J71" t="n">
-        <v>64.22491121292114</v>
+        <v>535.1971516609192</v>
       </c>
     </row>
     <row r="72">
@@ -2861,31 +2861,31 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>2809</v>
+        <v>3185</v>
       </c>
       <c r="C72" t="n">
         <v>1567</v>
       </c>
       <c r="D72" t="n">
-        <v>1342</v>
+        <v>1527</v>
       </c>
       <c r="E72" t="n">
-        <v>1466</v>
+        <v>1657</v>
       </c>
       <c r="F72" t="n">
-        <v>224</v>
+        <v>40</v>
       </c>
       <c r="G72" t="n">
-        <v>85.69604086845466</v>
+        <v>97.44735162731334</v>
       </c>
       <c r="H72" t="n">
-        <v>47.79202279202279</v>
+        <v>47.95854271356784</v>
       </c>
       <c r="I72" t="n">
-        <v>1.078493937460115</v>
+        <v>1.082961072112317</v>
       </c>
       <c r="J72" t="n">
-        <v>68.21327972412109</v>
+        <v>273.6702826023102</v>
       </c>
     </row>
     <row r="73">
@@ -2895,31 +2895,31 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>1667</v>
+        <v>1839</v>
       </c>
       <c r="C73" t="n">
         <v>920</v>
       </c>
       <c r="D73" t="n">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="E73" t="n">
-        <v>751</v>
+        <v>921</v>
       </c>
       <c r="F73" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G73" t="n">
-        <v>99.56474428726877</v>
+        <v>99.78237214363439</v>
       </c>
       <c r="H73" t="n">
-        <v>54.92196878751501</v>
+        <v>49.8911860718172</v>
       </c>
       <c r="I73" t="n">
-        <v>0.8206521739130435</v>
+        <v>1.003260869565217</v>
       </c>
       <c r="J73" t="n">
-        <v>64.56718516349792</v>
+        <v>391.3193991184235</v>
       </c>
     </row>
     <row r="74">
@@ -2929,31 +2929,31 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>2039</v>
+        <v>2314</v>
       </c>
       <c r="C74" t="n">
         <v>1143</v>
       </c>
       <c r="D74" t="n">
-        <v>1116</v>
+        <v>1127</v>
       </c>
       <c r="E74" t="n">
-        <v>922</v>
+        <v>1186</v>
       </c>
       <c r="F74" t="n">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="G74" t="n">
-        <v>97.72329246935202</v>
+        <v>98.68651488616463</v>
       </c>
       <c r="H74" t="n">
-        <v>54.75956820412168</v>
+        <v>48.72460008646779</v>
       </c>
       <c r="I74" t="n">
-        <v>0.8293963254593176</v>
+        <v>1.05074365704287</v>
       </c>
       <c r="J74" t="n">
-        <v>66.60217308998108</v>
+        <v>394.9015381336212</v>
       </c>
     </row>
     <row r="75">
@@ -2963,31 +2963,31 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>2613</v>
+        <v>3059</v>
       </c>
       <c r="C75" t="n">
         <v>1356</v>
       </c>
       <c r="D75" t="n">
-        <v>1153</v>
+        <v>1267</v>
       </c>
       <c r="E75" t="n">
-        <v>1459</v>
+        <v>1791</v>
       </c>
       <c r="F75" t="n">
-        <v>202</v>
+        <v>88</v>
       </c>
       <c r="G75" t="n">
-        <v>85.09225092250922</v>
+        <v>93.50553505535055</v>
       </c>
       <c r="H75" t="n">
-        <v>44.14241960183767</v>
+        <v>41.43230869849575</v>
       </c>
       <c r="I75" t="n">
-        <v>1.224926253687316</v>
+        <v>1.385693215339233</v>
       </c>
       <c r="J75" t="n">
-        <v>67.63453912734985</v>
+        <v>310.7905344963074</v>
       </c>
     </row>
     <row r="76">
@@ -2997,31 +2997,31 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>2584</v>
+        <v>2909</v>
       </c>
       <c r="C76" t="n">
         <v>543</v>
       </c>
       <c r="D76" t="n">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E76" t="n">
-        <v>2052</v>
+        <v>2375</v>
       </c>
       <c r="F76" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G76" t="n">
-        <v>97.97047970479704</v>
+        <v>98.33948339483395</v>
       </c>
       <c r="H76" t="n">
-        <v>20.55749128919861</v>
+        <v>18.32874828060523</v>
       </c>
       <c r="I76" t="n">
-        <v>3.79926335174954</v>
+        <v>4.390423572744015</v>
       </c>
       <c r="J76" t="n">
-        <v>67.06034731864929</v>
+        <v>351.3063015937805</v>
       </c>
     </row>
     <row r="77">
@@ -3031,31 +3031,31 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>2055</v>
+        <v>2108</v>
       </c>
       <c r="C77" t="n">
         <v>2025</v>
       </c>
       <c r="D77" t="n">
-        <v>1959</v>
+        <v>1990</v>
       </c>
       <c r="E77" t="n">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="F77" t="n">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="G77" t="n">
-        <v>96.78853754940711</v>
+        <v>98.3201581027668</v>
       </c>
       <c r="H77" t="n">
-        <v>95.37487828627069</v>
+        <v>94.44708115804461</v>
       </c>
       <c r="I77" t="n">
-        <v>0.07901234567901234</v>
+        <v>0.0745679012345679</v>
       </c>
       <c r="J77" t="n">
-        <v>63.12272906303406</v>
+        <v>419.7124400138855</v>
       </c>
     </row>
     <row r="78">
@@ -3065,7 +3065,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>2946</v>
+        <v>3180</v>
       </c>
       <c r="C78" t="n">
         <v>2145</v>
@@ -3074,7 +3074,7 @@
         <v>2144</v>
       </c>
       <c r="E78" t="n">
-        <v>801</v>
+        <v>1035</v>
       </c>
       <c r="F78" t="n">
         <v>0</v>
@@ -3083,13 +3083,13 @@
         <v>100</v>
       </c>
       <c r="H78" t="n">
-        <v>72.80135823429542</v>
+        <v>67.44259201006606</v>
       </c>
       <c r="I78" t="n">
-        <v>0.3734265734265734</v>
+        <v>0.4825174825174825</v>
       </c>
       <c r="J78" t="n">
-        <v>73.24848103523254</v>
+        <v>235.9911723136902</v>
       </c>
     </row>
   </sheetData>

</xml_diff>